<commit_message>
Add CMO Dashboard visualizations: scatter chart, bar chart, traffic lights
- Competitive Positioning Matrix (scatter) at H7: My Product vs Competitors
- High vs Low Segment Gap (bar chart) at H31: Awareness, Price, Attractiveness
- Traffic light icons for Awareness column (green >70%, yellow 40-70%, red <40%)
- Price Gap red text formatting when >10% above competitor
- Chart data tables in columns H-J
</commit_message>
<xml_diff>
--- a/CMO Dashboard/CMO_Dashboard_Complete.xlsx
+++ b/CMO Dashboard/CMO_Dashboard_Complete.xlsx
@@ -111,12 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -144,6 +145,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="009C0006"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -214,6 +223,316 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Competitive Positioning Matrix</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>My Product</v>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="12"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$I$4</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$J$4</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Competitors</v>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="diamond"/>
+            <size val="12"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$I$5</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$J$5</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Price ($)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Attractiveness Score</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>High vs Low Segment Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'SEGMENT_PULSE'!I26</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$H$27:$H$29</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$I$27:$I$29</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'SEGMENT_PULSE'!J26</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$H$27:$H$29</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'SEGMENT_PULSE'!$J$27:$J$29</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4320000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>30</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4320000" cy="3600000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,7 +824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +838,9 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="32" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -527,6 +849,11 @@
           <t>SEGMENT PULSE - Market Allocation Drivers</t>
         </is>
       </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>COMPETITIVE POSITIONING</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -534,6 +861,21 @@
           <t>HIGH SEGMENT ANALYSIS</t>
         </is>
       </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Entity</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Attractiveness</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -566,6 +908,17 @@
           <t>Allocation Flag</t>
         </is>
       </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>My Product</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -573,22 +926,33 @@
           <t>Center</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F5" s="7" t="inlineStr">
+      <c r="F5" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>Competitors</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -597,19 +961,19 @@
           <t>West</t>
         </is>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F6" s="7" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -621,19 +985,19 @@
           <t>North</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F7" s="7" t="inlineStr">
+      <c r="F7" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -645,19 +1009,19 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F8" s="7" t="inlineStr">
+      <c r="F8" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -669,19 +1033,19 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F9" s="7" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -732,19 +1096,19 @@
           <t>Center</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F14" s="7" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -756,19 +1120,19 @@
           <t>West</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F15" s="7" t="inlineStr">
+      <c r="F15" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -780,19 +1144,19 @@
           <t>North</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F16" s="7" t="inlineStr">
+      <c r="F16" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -804,19 +1168,19 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n">
+      <c r="B17" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F17" s="7" t="inlineStr">
+      <c r="F17" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -828,22 +1192,85 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n">
+      <c r="B18" s="6" t="n">
         <v>25</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F18" s="7" t="inlineStr">
+      <c r="F18" s="8" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>HIGH vs LOW SEGMENT GAP</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>High Segment</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>Low Segment</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="H27" s="4" t="inlineStr">
+        <is>
+          <t>Awareness</t>
+        </is>
+      </c>
+      <c r="I27" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="H28" s="4" t="inlineStr">
+        <is>
+          <t>Price Competitiveness</t>
+        </is>
+      </c>
+      <c r="I28" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J28" s="4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="H29" s="4" t="inlineStr">
+        <is>
+          <t>Attractiveness</t>
+        </is>
+      </c>
+      <c r="I29" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +1292,36 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C9">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3TrafficLights1" showValue="1" reverse="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="40"/>
+        <cfvo type="num" val="70"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C17">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3TrafficLights1" showValue="1" reverse="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="40"/>
+        <cfvo type="num" val="70"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D9">
+    <cfRule type="expression" priority="5" dxfId="0">
+      <formula>D5&gt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D17">
+    <cfRule type="expression" priority="5" dxfId="0">
+      <formula>D5&gt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -896,7 +1352,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Note: Innovations increase Attractiveness. Required for High Segment Allocation.</t>
         </is>
@@ -925,10 +1381,10 @@
           <t>STAINLESS MATERIAL</t>
         </is>
       </c>
-      <c r="B5" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="n">
+      <c r="B5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -938,10 +1394,10 @@
           <t>RECYCLABLE MATERIALS</t>
         </is>
       </c>
-      <c r="B6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10" t="n">
+      <c r="B6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -951,10 +1407,10 @@
           <t>ENERGY EFFICIENCY</t>
         </is>
       </c>
-      <c r="B7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10" t="n">
+      <c r="B7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -964,10 +1420,10 @@
           <t>LIGHTER AND MORE COMPACT</t>
         </is>
       </c>
-      <c r="B8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10" t="n">
+      <c r="B8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -977,10 +1433,10 @@
           <t>IMPACT RESISTANCE</t>
         </is>
       </c>
-      <c r="B9" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="n">
+      <c r="B9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -990,10 +1446,10 @@
           <t>NOISE REDUCTION</t>
         </is>
       </c>
-      <c r="B10" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10" t="n">
+      <c r="B10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1003,10 +1459,10 @@
           <t>IMPROVED BATTERY CAPACITY</t>
         </is>
       </c>
-      <c r="B11" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10" t="n">
+      <c r="B11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1016,10 +1472,10 @@
           <t>SELF-CLEANING</t>
         </is>
       </c>
-      <c r="B12" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10" t="n">
+      <c r="B12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1029,10 +1485,10 @@
           <t>SPEED SETTINGS</t>
         </is>
       </c>
-      <c r="B13" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="10" t="n">
+      <c r="B13" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1042,10 +1498,10 @@
           <t>DIGITAL CONTROLS</t>
         </is>
       </c>
-      <c r="B14" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="10" t="n">
+      <c r="B14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1055,10 +1511,10 @@
           <t>VOICE ASSISTANCE INTEGRATION</t>
         </is>
       </c>
-      <c r="B15" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="10" t="n">
+      <c r="B15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1068,10 +1524,10 @@
           <t>AUTOMATION AND PROGRAMMABILITY</t>
         </is>
       </c>
-      <c r="B16" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="10" t="n">
+      <c r="B16" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1081,10 +1537,10 @@
           <t>MULTIFUNCTIONAL ACCESSORIES</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="10" t="n">
+      <c r="B17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1094,20 +1550,20 @@
           <t>MAPPING TECHNOLOGY</t>
         </is>
       </c>
-      <c r="B18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="10" t="n">
+      <c r="B18" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="inlineStr">
+      <c r="A20" s="12" t="inlineStr">
         <is>
           <t>TOTAL INNOVATION COST</t>
         </is>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="13">
         <f>SUMPRODUCT(B5:B18,C5:C18)</f>
         <v/>
       </c>
@@ -1145,7 +1601,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>HOW TO USE: Adjust Yellow cells. Check Profit Projection. Go to UPLOAD_READY tabs to copy decisions.</t>
         </is>
@@ -1164,10 +1620,10 @@
           <t>TV Budget ($)</t>
         </is>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="11" t="n">
         <v>35</v>
       </c>
-      <c r="C5" s="8" t="inlineStr">
+      <c r="C5" s="9" t="inlineStr">
         <is>
           <t>Primary Driver: High Segment Awareness</t>
         </is>
@@ -1179,10 +1635,10 @@
           <t>Brand Focus (0-100)</t>
         </is>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="C6" s="8" t="inlineStr">
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>0=Awareness focus, 100=Attributes focus</t>
         </is>
@@ -1196,57 +1652,57 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="14" t="inlineStr">
+      <c r="A11" s="15" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="B11" s="14" t="inlineStr">
+      <c r="B11" s="15" t="inlineStr">
         <is>
           <t>Last Sales</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr">
+      <c r="C11" s="15" t="inlineStr">
         <is>
           <t>Stockout?</t>
         </is>
       </c>
-      <c r="D11" s="14" t="inlineStr">
+      <c r="D11" s="15" t="inlineStr">
         <is>
           <t>Target Demand</t>
         </is>
       </c>
-      <c r="E11" s="14" t="inlineStr">
+      <c r="E11" s="15" t="inlineStr">
         <is>
           <t>Radio Budget</t>
         </is>
       </c>
-      <c r="F11" s="14" t="inlineStr">
+      <c r="F11" s="15" t="inlineStr">
         <is>
           <t>Salespeople</t>
         </is>
       </c>
-      <c r="G11" s="14" t="inlineStr">
+      <c r="G11" s="15" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="H11" s="14" t="inlineStr">
+      <c r="H11" s="15" t="inlineStr">
         <is>
           <t>Payment</t>
         </is>
       </c>
-      <c r="I11" s="14" t="inlineStr">
+      <c r="I11" s="15" t="inlineStr">
         <is>
           <t>Est. Revenue</t>
         </is>
       </c>
-      <c r="J11" s="14" t="inlineStr">
+      <c r="J11" s="15" t="inlineStr">
         <is>
           <t>Mkt Cost</t>
         </is>
       </c>
-      <c r="K11" s="14" t="inlineStr">
+      <c r="K11" s="15" t="inlineStr">
         <is>
           <t>Contribution</t>
         </is>
@@ -1258,40 +1714,40 @@
           <t>Center</t>
         </is>
       </c>
-      <c r="B12" s="15" t="n">
+      <c r="B12" s="16" t="n">
         <v>1000</v>
       </c>
-      <c r="C12" s="16" t="inlineStr">
+      <c r="C12" s="17" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="D12" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="11" t="n">
         <v>210</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F12" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="H12" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="19">
         <f>D12*G12</f>
         <v/>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="19">
         <f>($B$5/5)+E12+(F12*5000)+(INNOVATION_LAB!C20/5)</f>
         <v/>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="20">
         <f>I12-J12-(D12*40)</f>
         <v/>
       </c>
@@ -1302,40 +1758,40 @@
           <t>West</t>
         </is>
       </c>
-      <c r="B13" s="15" t="n">
+      <c r="B13" s="16" t="n">
         <v>1000</v>
       </c>
-      <c r="C13" s="16" t="inlineStr">
+      <c r="C13" s="17" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="D13" s="17" t="n">
+      <c r="D13" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="E13" s="10" t="n">
+      <c r="E13" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="F13" s="13" t="n">
+      <c r="F13" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="H13" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="19">
         <f>D13*G13</f>
         <v/>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="19">
         <f>($B$5/5)+E13+(F13*5000)+(INNOVATION_LAB!C20/5)</f>
         <v/>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="20">
         <f>I13-J13-(D13*40)</f>
         <v/>
       </c>
@@ -1346,40 +1802,40 @@
           <t>North</t>
         </is>
       </c>
-      <c r="B14" s="15" t="n">
+      <c r="B14" s="16" t="n">
         <v>1000</v>
       </c>
-      <c r="C14" s="16" t="inlineStr">
+      <c r="C14" s="17" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="D14" s="17" t="n">
+      <c r="D14" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="11" t="n">
         <v>82</v>
       </c>
-      <c r="F14" s="13" t="n">
+      <c r="F14" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="H14" s="9" t="inlineStr">
+      <c r="H14" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="19">
         <f>D14*G14</f>
         <v/>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="19">
         <f>($B$5/5)+E14+(F14*5000)+(INNOVATION_LAB!C20/5)</f>
         <v/>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="20">
         <f>I14-J14-(D14*40)</f>
         <v/>
       </c>
@@ -1390,40 +1846,40 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B15" s="15" t="n">
+      <c r="B15" s="16" t="n">
         <v>1000</v>
       </c>
-      <c r="C15" s="16" t="inlineStr">
+      <c r="C15" s="17" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="D15" s="17" t="n">
+      <c r="D15" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="H15" s="9" t="inlineStr">
+      <c r="H15" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="19">
         <f>D15*G15</f>
         <v/>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="19">
         <f>($B$5/5)+E15+(F15*5000)+(INNOVATION_LAB!C20/5)</f>
         <v/>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="20">
         <f>I15-J15-(D15*40)</f>
         <v/>
       </c>
@@ -1434,63 +1890,63 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B16" s="15" t="n">
+      <c r="B16" s="16" t="n">
         <v>1000</v>
       </c>
-      <c r="C16" s="16" t="inlineStr">
+      <c r="C16" s="17" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="D16" s="17" t="n">
+      <c r="D16" s="18" t="n">
         <v>1000</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="E16" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="F16" s="13" t="n">
+      <c r="F16" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G16" s="10" t="n">
+      <c r="G16" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="H16" s="9" t="inlineStr">
+      <c r="H16" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="19">
         <f>D16*G16</f>
         <v/>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="19">
         <f>($B$5/5)+E16+(F16*5000)+(INNOVATION_LAB!C20/5)</f>
         <v/>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="20">
         <f>I16-J16-(D16*40)</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="inlineStr">
+      <c r="A17" s="12" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="21">
         <f>SUM(D12:D16)</f>
         <v/>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="22">
         <f>SUM(I12:I16)</f>
         <v/>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="22">
         <f>SUM(J12:J16)</f>
         <v/>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="23">
         <f>SUM(K12:K16)</f>
         <v/>
       </c>
@@ -1522,7 +1978,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Copy these values to ExSim Marketing upload</t>
         </is>
@@ -1576,42 +2032,42 @@
           <t>Brand Focus</t>
         </is>
       </c>
-      <c r="G5" s="23" t="inlineStr">
+      <c r="G5" s="24" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="H5" s="23" t="inlineStr">
+      <c r="H5" s="24" t="inlineStr">
         <is>
           <t>Demand</t>
         </is>
       </c>
-      <c r="J5" s="23" t="inlineStr">
+      <c r="J5" s="24" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="K5" s="23" t="inlineStr">
+      <c r="K5" s="24" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="L5" s="23" t="inlineStr">
+      <c r="L5" s="24" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="N5" s="23" t="inlineStr">
+      <c r="N5" s="24" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="O5" s="23" t="inlineStr">
+      <c r="O5" s="24" t="inlineStr">
         <is>
           <t>Payment</t>
         </is>
       </c>
-      <c r="P5" s="23" t="inlineStr">
+      <c r="P5" s="24" t="inlineStr">
         <is>
           <t>Salespeople</t>
         </is>
@@ -1979,24 +2435,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Copy these values to ExSim Innovation upload</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="inlineStr">
+      <c r="A4" s="24" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B4" s="23" t="inlineStr">
+      <c r="B4" s="24" t="inlineStr">
         <is>
           <t>Improvement</t>
         </is>
       </c>
-      <c r="C4" s="23" t="inlineStr">
+      <c r="C4" s="24" t="inlineStr">
         <is>
           <t>Value</t>
         </is>

</xml_diff>

<commit_message>
Update dashboards, War Room tabs, and shared output logic
</commit_message>
<xml_diff>
--- a/CMO Dashboard/CMO_Dashboard_Complete.xlsx
+++ b/CMO Dashboard/CMO_Dashboard_Complete.xlsx
@@ -96,6 +96,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFF2CC"/>
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
@@ -110,12 +116,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00E7E6E6"/>
         <bgColor rgb="00E7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D9D9D9"/>
-        <bgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -150,24 +150,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="5" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -1085,9 +1086,9 @@
       <c r="F8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="11" t="inlineStr">
-        <is>
-          <t>CRITICAL: Boost TV for Allocation</t>
+      <c r="G8" s="12" t="inlineStr">
+        <is>
+          <t>NO PRESENCE: Zone Not Active</t>
         </is>
       </c>
     </row>
@@ -1112,9 +1113,9 @@
       <c r="F9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="11" t="inlineStr">
-        <is>
-          <t>CRITICAL: Boost TV for Allocation</t>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>NO PRESENCE: Zone Not Active</t>
         </is>
       </c>
     </row>
@@ -1183,7 +1184,7 @@
       <c r="F14" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G14" s="12" t="inlineStr">
+      <c r="G14" s="13" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1210,7 +1211,7 @@
       <c r="F15" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G15" s="12" t="inlineStr">
+      <c r="G15" s="13" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1237,7 +1238,7 @@
       <c r="F16" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G16" s="12" t="inlineStr">
+      <c r="G16" s="13" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1266,7 +1267,7 @@
       </c>
       <c r="G17" s="12" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>NO PRESENCE: Zone Not Active</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1294,7 @@
       </c>
       <c r="G18" s="12" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>NO PRESENCE: Zone Not Active</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1441,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="inlineStr">
+      <c r="A2" s="14" t="inlineStr">
         <is>
           <t>Note: Innovations increase Attractiveness. Required for High Segment Allocation.</t>
         </is>
@@ -1474,13 +1475,13 @@
           <t>STAINLESS MATERIAL</t>
         </is>
       </c>
-      <c r="B5" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="15" t="n">
+      <c r="B5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="17">
         <f>C5</f>
         <v/>
       </c>
@@ -1491,13 +1492,13 @@
           <t>RECYCLABLE MATERIALS</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="15" t="n">
+      <c r="B6" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="17">
         <f>C6</f>
         <v/>
       </c>
@@ -1508,13 +1509,13 @@
           <t>ENERGY EFFICIENCY</t>
         </is>
       </c>
-      <c r="B7" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="15" t="n">
+      <c r="B7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="17">
         <f>C7</f>
         <v/>
       </c>
@@ -1525,13 +1526,13 @@
           <t>LIGHTER AND MORE COMPACT</t>
         </is>
       </c>
-      <c r="B8" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="15" t="n">
+      <c r="B8" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="17">
         <f>C8</f>
         <v/>
       </c>
@@ -1542,13 +1543,13 @@
           <t>IMPACT RESISTANCE</t>
         </is>
       </c>
-      <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="n">
+      <c r="B9" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="17">
         <f>C9</f>
         <v/>
       </c>
@@ -1559,13 +1560,13 @@
           <t>NOISE REDUCTION</t>
         </is>
       </c>
-      <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="n">
+      <c r="B10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="17">
         <f>C10</f>
         <v/>
       </c>
@@ -1576,13 +1577,13 @@
           <t>IMPROVED BATTERY CAPACITY</t>
         </is>
       </c>
-      <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="n">
+      <c r="B11" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="17">
         <f>C11</f>
         <v/>
       </c>
@@ -1593,13 +1594,13 @@
           <t>SELF-CLEANING</t>
         </is>
       </c>
-      <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="n">
+      <c r="B12" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="17">
         <f>C12</f>
         <v/>
       </c>
@@ -1610,13 +1611,13 @@
           <t>SPEED SETTINGS</t>
         </is>
       </c>
-      <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="n">
+      <c r="B13" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="17">
         <f>C13</f>
         <v/>
       </c>
@@ -1627,13 +1628,13 @@
           <t>DIGITAL CONTROLS</t>
         </is>
       </c>
-      <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="n">
+      <c r="B14" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="17">
         <f>C14</f>
         <v/>
       </c>
@@ -1644,13 +1645,13 @@
           <t>VOICE ASSISTANCE INTEGRATION</t>
         </is>
       </c>
-      <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="n">
+      <c r="B15" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="17">
         <f>C15</f>
         <v/>
       </c>
@@ -1661,13 +1662,13 @@
           <t>AUTOMATION AND PROGRAMMABILITY</t>
         </is>
       </c>
-      <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="n">
+      <c r="B16" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="17">
         <f>C16</f>
         <v/>
       </c>
@@ -1678,13 +1679,13 @@
           <t>MULTIFUNCTIONAL ACCESSORIES</t>
         </is>
       </c>
-      <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="n">
+      <c r="B17" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="17">
         <f>C17</f>
         <v/>
       </c>
@@ -1695,24 +1696,24 @@
           <t>MAPPING TECHNOLOGY</t>
         </is>
       </c>
-      <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="n">
+      <c r="B18" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="n">
         <v>10000</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="17">
         <f>C18</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="17" t="inlineStr">
+      <c r="A20" s="18" t="inlineStr">
         <is>
           <t>TOTAL INNOVATION COST</t>
         </is>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="19">
         <f>SUMPRODUCT(B5:B18,C5:C18)</f>
         <v/>
       </c>
@@ -1762,43 +1763,43 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="inlineStr">
+      <c r="A2" s="20" t="inlineStr">
         <is>
           <t>TV Cost/Spot</t>
         </is>
       </c>
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B2" s="20" t="inlineStr">
         <is>
           <t>Radio Cost/Spot</t>
         </is>
       </c>
-      <c r="C2" s="19" t="inlineStr">
+      <c r="C2" s="20" t="inlineStr">
         <is>
           <t>Hiring Fee</t>
         </is>
       </c>
-      <c r="D2" s="19" t="inlineStr">
+      <c r="D2" s="20" t="inlineStr">
         <is>
           <t>Salary/Person</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="n">
+      <c r="A3" s="21" t="n">
         <v>3000</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="21" t="n">
         <v>300</v>
       </c>
-      <c r="C3" s="20" t="n">
+      <c r="C3" s="21" t="n">
         <v>1100</v>
       </c>
-      <c r="D3" s="20" t="n">
+      <c r="D3" s="21" t="n">
         <v>1500</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="inlineStr">
+      <c r="A5" s="14" t="inlineStr">
         <is>
           <t>HOW TO USE: Adjust Yellow cells. Check Profit Projection. Go to UPLOAD_READY tabs to copy decisions.</t>
         </is>
@@ -1817,10 +1818,10 @@
           <t>TV Spots (Qty)</t>
         </is>
       </c>
-      <c r="B9" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17">
         <f>B9*3000.0</f>
         <v/>
       </c>
@@ -1831,10 +1832,10 @@
           <t>Brand Focus (0-100)</t>
         </is>
       </c>
-      <c r="B10" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="13" t="inlineStr">
+      <c r="B10" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14" t="inlineStr">
         <is>
           <t>0=Awareness focus, 100=Attributes focus</t>
         </is>
@@ -1848,62 +1849,62 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="22" t="inlineStr">
+      <c r="A15" s="23" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="B15" s="22" t="inlineStr">
+      <c r="B15" s="23" t="inlineStr">
         <is>
           <t>Last Sales</t>
         </is>
       </c>
-      <c r="C15" s="22" t="inlineStr">
+      <c r="C15" s="23" t="inlineStr">
         <is>
           <t>Stockout?</t>
         </is>
       </c>
-      <c r="D15" s="22" t="inlineStr">
+      <c r="D15" s="23" t="inlineStr">
         <is>
           <t>Target Demand</t>
         </is>
       </c>
-      <c r="E15" s="22" t="inlineStr">
+      <c r="E15" s="23" t="inlineStr">
         <is>
           <t>Radio Spots (Qty)</t>
         </is>
       </c>
-      <c r="F15" s="22" t="inlineStr">
+      <c r="F15" s="23" t="inlineStr">
         <is>
           <t>Headcount</t>
         </is>
       </c>
-      <c r="G15" s="22" t="inlineStr">
+      <c r="G15" s="23" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="H15" s="22" t="inlineStr">
+      <c r="H15" s="23" t="inlineStr">
         <is>
           <t>Avg Comp Price</t>
         </is>
       </c>
-      <c r="I15" s="22" t="inlineStr">
+      <c r="I15" s="23" t="inlineStr">
         <is>
           <t>Payment</t>
         </is>
       </c>
-      <c r="J15" s="22" t="inlineStr">
+      <c r="J15" s="23" t="inlineStr">
         <is>
           <t>Est. Revenue</t>
         </is>
       </c>
-      <c r="K15" s="22" t="inlineStr">
+      <c r="K15" s="23" t="inlineStr">
         <is>
           <t>Mkt Cost</t>
         </is>
       </c>
-      <c r="L15" s="22" t="inlineStr">
+      <c r="L15" s="23" t="inlineStr">
         <is>
           <t>Contribution</t>
         </is>
@@ -1915,39 +1916,39 @@
           <t>Center</t>
         </is>
       </c>
-      <c r="B16" s="23" t="n">
+      <c r="B16" s="24" t="n">
         <v>8900</v>
       </c>
-      <c r="C16" s="24" t="inlineStr">
+      <c r="C16" s="25" t="inlineStr">
         <is>
           <t>TRUE DEMAND HIGHER</t>
         </is>
       </c>
-      <c r="D16" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="25" t="n">
+      <c r="D16" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="26" t="n">
         <v>68</v>
       </c>
-      <c r="I16" s="21" t="inlineStr"/>
-      <c r="J16" s="16">
+      <c r="I16" s="22" t="inlineStr"/>
+      <c r="J16" s="17">
         <f>D16*G16</f>
         <v/>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="17">
         <f>(C9/5) + (E16*300.0) + (F16*1500) + (MAX(0, F16-5)*1100)</f>
         <v/>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="27">
         <f>J16-K16</f>
         <v/>
       </c>
@@ -1958,39 +1959,39 @@
           <t>West</t>
         </is>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="24" t="n">
         <v>4028</v>
       </c>
-      <c r="C17" s="24" t="inlineStr">
+      <c r="C17" s="25" t="inlineStr">
         <is>
           <t>TRUE DEMAND HIGHER</t>
         </is>
       </c>
-      <c r="D17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="25" t="n">
+      <c r="D17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="26" t="n">
         <v>68</v>
       </c>
-      <c r="I17" s="21" t="inlineStr"/>
-      <c r="J17" s="16">
+      <c r="I17" s="22" t="inlineStr"/>
+      <c r="J17" s="17">
         <f>D17*G17</f>
         <v/>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="17">
         <f>(C9/5) + (E17*300.0) + (F17*1500) + (MAX(0, F17-5)*1100)</f>
         <v/>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="27">
         <f>J17-K17</f>
         <v/>
       </c>
@@ -2001,39 +2002,39 @@
           <t>North</t>
         </is>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="24" t="n">
         <v>4400</v>
       </c>
-      <c r="C18" s="24" t="inlineStr">
+      <c r="C18" s="25" t="inlineStr">
         <is>
           <t>TRUE DEMAND HIGHER</t>
         </is>
       </c>
-      <c r="D18" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="25" t="n">
+      <c r="D18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="26" t="n">
         <v>91</v>
       </c>
-      <c r="I18" s="21" t="inlineStr"/>
-      <c r="J18" s="16">
+      <c r="I18" s="22" t="inlineStr"/>
+      <c r="J18" s="17">
         <f>D18*G18</f>
         <v/>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="17">
         <f>(C9/5) + (E18*300.0) + (F18*1500) + (MAX(0, F18-5)*1100)</f>
         <v/>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="27">
         <f>J18-K18</f>
         <v/>
       </c>
@@ -2044,39 +2045,39 @@
           <t>East</t>
         </is>
       </c>
-      <c r="B19" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="24" t="inlineStr">
+      <c r="B19" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="25" t="inlineStr">
         <is>
           <t>TRUE DEMAND HIGHER</t>
         </is>
       </c>
-      <c r="D19" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="21" t="inlineStr"/>
-      <c r="J19" s="16">
+      <c r="D19" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="22" t="inlineStr"/>
+      <c r="J19" s="17">
         <f>D19*G19</f>
         <v/>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="17">
         <f>(C9/5) + (E19*300.0) + (F19*1500) + (MAX(0, F19-5)*1100)</f>
         <v/>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="27">
         <f>J19-K19</f>
         <v/>
       </c>
@@ -2087,39 +2088,39 @@
           <t>South</t>
         </is>
       </c>
-      <c r="B20" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="24" t="inlineStr">
+      <c r="B20" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="25" t="inlineStr">
         <is>
           <t>TRUE DEMAND HIGHER</t>
         </is>
       </c>
-      <c r="D20" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="21" t="inlineStr"/>
-      <c r="J20" s="16">
+      <c r="D20" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="22" t="inlineStr"/>
+      <c r="J20" s="17">
         <f>D20*G20</f>
         <v/>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="17">
         <f>(C9/5) + (E20*300.0) + (F20*1500) + (MAX(0, F20-5)*1100)</f>
         <v/>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="27">
         <f>J20-K20</f>
         <v/>
       </c>
@@ -2176,7 +2177,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="inlineStr">
+      <c r="A2" s="14" t="inlineStr">
         <is>
           <t>Copy these values to ExSim Marketing upload</t>
         </is>
@@ -2230,42 +2231,42 @@
           <t>Brand Focus</t>
         </is>
       </c>
-      <c r="G5" s="27" t="inlineStr">
+      <c r="G5" s="28" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="H5" s="27" t="inlineStr">
+      <c r="H5" s="28" t="inlineStr">
         <is>
           <t>Demand</t>
         </is>
       </c>
-      <c r="J5" s="27" t="inlineStr">
+      <c r="J5" s="28" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="K5" s="27" t="inlineStr">
+      <c r="K5" s="28" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="L5" s="27" t="inlineStr">
+      <c r="L5" s="28" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="N5" s="27" t="inlineStr">
+      <c r="N5" s="28" t="inlineStr">
         <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="O5" s="27" t="inlineStr">
+      <c r="O5" s="28" t="inlineStr">
         <is>
           <t>Payment</t>
         </is>
       </c>
-      <c r="P5" s="27" t="inlineStr">
+      <c r="P5" s="28" t="inlineStr">
         <is>
           <t>Salespeople</t>
         </is>
@@ -2633,24 +2634,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="inlineStr">
+      <c r="A2" s="14" t="inlineStr">
         <is>
           <t>Copy these values to ExSim Innovation upload</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27" t="inlineStr">
+      <c r="A4" s="28" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B4" s="27" t="inlineStr">
+      <c r="B4" s="28" t="inlineStr">
         <is>
           <t>Improvement</t>
         </is>
       </c>
-      <c r="C4" s="27" t="inlineStr">
+      <c r="C4" s="28" t="inlineStr">
         <is>
           <t>Value</t>
         </is>

</xml_diff>